<commit_message>
Edit Text Buyer Pages UI
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Core\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC1F62-CE86-498F-98A2-E2B5AA882D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A7687-FBAC-4D1E-8A4A-BE4454ED3B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1785" windowWidth="21600" windowHeight="11115" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
+    <workbookView xWindow="28680" yWindow="1215" windowWidth="20730" windowHeight="11760" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Onboarding" sheetId="11" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="1381">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -4085,9 +4085,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>arcadierteam@gmail.com</t>
-  </si>
-  <si>
     <t>C:\\Katalon\\Arctick\\Images\\LogoLayout\\logo1.jpg</t>
   </si>
   <si>
@@ -4182,6 +4179,12 @@
   </si>
   <si>
     <t>0723OMP</t>
+  </si>
+  <si>
+    <t>arcqatester01@gmail.com</t>
+  </si>
+  <si>
+    <t>09296monthsscale01</t>
   </si>
 </sst>
 </file>
@@ -4866,8 +4869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEEA25A-B9EE-4434-8603-4CD75E6C0C65}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4955,13 +4958,13 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="30" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>976</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>968</v>
@@ -4976,25 +4979,25 @@
         <v>971</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="M2" s="30" t="s">
         <v>972</v>
       </c>
       <c r="N2" s="32" t="s">
+        <v>1379</v>
+      </c>
+      <c r="O2" s="32" t="s">
         <v>1347</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="P2" s="32" t="s">
         <v>1348</v>
       </c>
-      <c r="P2" s="32" t="s">
-        <v>1349</v>
-      </c>
       <c r="Q2" s="33" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="S2" s="30" t="s">
         <v>1000</v>
@@ -5006,8 +5009,11 @@
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{96F17C4C-075C-47DF-8309-62D10E27B300}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11520,7 +11526,7 @@
         <v>1010</v>
       </c>
       <c r="K20" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M20" t="s">
         <v>1173</v>
@@ -11570,7 +11576,7 @@
         <v>1010</v>
       </c>
       <c r="K21" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M21" t="s">
         <v>1174</v>
@@ -11620,7 +11626,7 @@
         <v>1237</v>
       </c>
       <c r="K22" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M22" t="s">
         <v>1175</v>
@@ -11670,7 +11676,7 @@
         <v>1010</v>
       </c>
       <c r="K23" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M23" t="s">
         <v>1176</v>
@@ -11726,7 +11732,7 @@
         <v>1010</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M24" t="s">
         <v>1177</v>
@@ -11776,7 +11782,7 @@
         <v>1010</v>
       </c>
       <c r="K25" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M25" t="s">
         <v>1178</v>
@@ -11826,7 +11832,7 @@
         <v>1237</v>
       </c>
       <c r="K26" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M26" t="s">
         <v>1179</v>
@@ -11876,7 +11882,7 @@
         <v>1010</v>
       </c>
       <c r="K27" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M27" t="s">
         <v>1180</v>
@@ -11926,7 +11932,7 @@
         <v>1330</v>
       </c>
       <c r="K28" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M28" t="s">
         <v>1181</v>
@@ -11973,7 +11979,7 @@
         <v>1010</v>
       </c>
       <c r="K29" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M29" t="s">
         <v>1182</v>
@@ -12020,7 +12026,7 @@
         <v>1010</v>
       </c>
       <c r="K30" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M30" t="s">
         <v>1183</v>
@@ -12067,7 +12073,7 @@
         <v>1010</v>
       </c>
       <c r="K31" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M31" t="s">
         <v>1184</v>
@@ -12114,7 +12120,7 @@
         <v>1010</v>
       </c>
       <c r="K32" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M32" t="s">
         <v>1185</v>
@@ -12161,7 +12167,7 @@
         <v>1010</v>
       </c>
       <c r="K33" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M33" t="s">
         <v>1186</v>
@@ -14683,7 +14689,7 @@
         <v>1067</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>161</v>
@@ -14730,7 +14736,7 @@
         <v>1068</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>168</v>
@@ -14777,7 +14783,7 @@
         <v>1069</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>173</v>
@@ -14822,7 +14828,7 @@
         <v>1070</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>178</v>
@@ -14869,7 +14875,7 @@
         <v>1071</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>185</v>
@@ -14916,7 +14922,7 @@
         <v>1072</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>192</v>
@@ -14963,7 +14969,7 @@
         <v>1073</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>198</v>
@@ -15010,7 +15016,7 @@
         <v>1074</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>203</v>
@@ -15057,7 +15063,7 @@
         <v>1075</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>208</v>
@@ -15104,7 +15110,7 @@
         <v>1076</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>212</v>
@@ -15151,7 +15157,7 @@
         <v>1077</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>217</v>
@@ -15198,7 +15204,7 @@
         <v>1078</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>222</v>
@@ -15245,7 +15251,7 @@
         <v>1079</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>227</v>
@@ -15292,7 +15298,7 @@
         <v>1080</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>232</v>
@@ -15339,7 +15345,7 @@
         <v>1081</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>238</v>
@@ -15386,7 +15392,7 @@
         <v>1082</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>243</v>
@@ -15433,7 +15439,7 @@
         <v>1083</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>248</v>
@@ -15480,7 +15486,7 @@
         <v>1084</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>253</v>
@@ -15525,7 +15531,7 @@
         <v>1085</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>257</v>
@@ -15570,7 +15576,7 @@
         <v>1086</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>264</v>
@@ -15615,7 +15621,7 @@
         <v>1087</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>269</v>
@@ -15660,7 +15666,7 @@
         <v>1088</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>275</v>
@@ -15815,7 +15821,7 @@
         <v>1067</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>281</v>
@@ -16718,7 +16724,7 @@
         <v>1206</v>
       </c>
       <c r="C2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>1207</v>
@@ -16774,7 +16780,7 @@
         <v>1212</v>
       </c>
       <c r="C3" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1213</v>
@@ -16828,7 +16834,7 @@
         <v>1218</v>
       </c>
       <c r="C4" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>1219</v>
@@ -16882,7 +16888,7 @@
         <v>1222</v>
       </c>
       <c r="C5" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>1223</v>
@@ -16936,7 +16942,7 @@
         <v>1228</v>
       </c>
       <c r="C6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>976</v>
@@ -16993,7 +16999,7 @@
         <v>1236</v>
       </c>
       <c r="C7" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>976</v>
@@ -17053,7 +17059,7 @@
         <v>1240</v>
       </c>
       <c r="C8" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>976</v>
@@ -17110,7 +17116,7 @@
         <v>1244</v>
       </c>
       <c r="C9" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>976</v>
@@ -17170,7 +17176,7 @@
         <v>1249</v>
       </c>
       <c r="C10" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>976</v>
@@ -17227,7 +17233,7 @@
         <v>1253</v>
       </c>
       <c r="C11" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>976</v>
@@ -17287,7 +17293,7 @@
         <v>1257</v>
       </c>
       <c r="C12" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>1207</v>
@@ -17341,7 +17347,7 @@
         <v>1263</v>
       </c>
       <c r="C13" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D13" s="48" t="s">
         <v>1213</v>
@@ -17395,7 +17401,7 @@
         <v>1265</v>
       </c>
       <c r="C14" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>1219</v>
@@ -17449,7 +17455,7 @@
         <v>1268</v>
       </c>
       <c r="C15" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>1223</v>
@@ -17503,7 +17509,7 @@
         <v>1270</v>
       </c>
       <c r="C16" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>976</v>
@@ -17562,7 +17568,7 @@
         <v>1276</v>
       </c>
       <c r="C17" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>976</v>
@@ -17624,7 +17630,7 @@
         <v>1281</v>
       </c>
       <c r="C18" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>976</v>
@@ -17683,7 +17689,7 @@
         <v>1286</v>
       </c>
       <c r="C19" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>976</v>
@@ -17742,7 +17748,7 @@
         <v>1291</v>
       </c>
       <c r="C20" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D20" s="2"/>
       <c r="G20" s="3">
@@ -17755,7 +17761,7 @@
         <v>1010</v>
       </c>
       <c r="K20" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M20" t="s">
         <v>1173</v>
@@ -17790,7 +17796,7 @@
         <v>1295</v>
       </c>
       <c r="C21" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>1219</v>
@@ -17805,7 +17811,7 @@
         <v>1010</v>
       </c>
       <c r="K21" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M21" t="s">
         <v>1174</v>
@@ -17840,7 +17846,7 @@
         <v>1299</v>
       </c>
       <c r="C22" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>1223</v>
@@ -17855,7 +17861,7 @@
         <v>1237</v>
       </c>
       <c r="K22" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M22" t="s">
         <v>1175</v>
@@ -17890,7 +17896,7 @@
         <v>1303</v>
       </c>
       <c r="C23" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>976</v>
@@ -17905,7 +17911,7 @@
         <v>1010</v>
       </c>
       <c r="K23" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M23" t="s">
         <v>1176</v>
@@ -17940,7 +17946,7 @@
         <v>1308</v>
       </c>
       <c r="C24" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>1309</v>
@@ -17961,7 +17967,7 @@
         <v>1010</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M24" t="s">
         <v>1177</v>
@@ -18011,7 +18017,7 @@
         <v>1010</v>
       </c>
       <c r="K25" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M25" t="s">
         <v>1178</v>
@@ -18061,7 +18067,7 @@
         <v>1237</v>
       </c>
       <c r="K26" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M26" t="s">
         <v>1179</v>
@@ -18111,7 +18117,7 @@
         <v>1010</v>
       </c>
       <c r="K27" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M27" t="s">
         <v>1180</v>
@@ -18161,7 +18167,7 @@
         <v>1330</v>
       </c>
       <c r="K28" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M28" t="s">
         <v>1181</v>
@@ -18208,7 +18214,7 @@
         <v>1010</v>
       </c>
       <c r="K29" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M29" t="s">
         <v>1182</v>
@@ -18255,7 +18261,7 @@
         <v>1010</v>
       </c>
       <c r="K30" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M30" t="s">
         <v>1183</v>
@@ -18302,7 +18308,7 @@
         <v>1010</v>
       </c>
       <c r="K31" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M31" t="s">
         <v>1184</v>
@@ -18349,7 +18355,7 @@
         <v>1010</v>
       </c>
       <c r="K32" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M32" t="s">
         <v>1185</v>
@@ -18396,7 +18402,7 @@
         <v>1010</v>
       </c>
       <c r="K33" s="55" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M33" t="s">
         <v>1186</v>

</xml_diff>